<commit_message>
FRET Verbesserung Bilder SE, E
</commit_message>
<xml_diff>
--- a/Versuch_FRET/04-Versuchsauswertung/Paul/42.xlsx
+++ b/Versuch_FRET/04-Versuchsauswertung/Paul/42.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/GitHub/PhyPraktikum/Versuch_FRET/04-Versuchsauswertung/Paul/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A989E7E-6413-1C4A-8AD4-B4C8AA91BB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE6FF5F-1958-5840-90AC-BFE244EECE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" activeTab="2" xr2:uid="{6D0E4EF2-1775-E943-B6E8-1DDB3097DE63}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" activeTab="1" xr2:uid="{6D0E4EF2-1775-E943-B6E8-1DDB3097DE63}"/>
   </bookViews>
   <sheets>
     <sheet name="SE-E-CY" sheetId="3" r:id="rId1"/>
@@ -1104,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC85BF5-D058-0D41-B40B-CDD072D3FB19}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1683,7 +1683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED7B5BDB-BCB4-0F48-B978-12681CAD4977}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>